<commit_message>
DOMA-746 add executor & assignee excel export mappers
</commit_message>
<xml_diff>
--- a/apps/condo/domains/ticket/templates/en/TicketAnalyticsExportTemplate[property_status].xlsx
+++ b/apps/condo/domains/ticket/templates/en/TicketAnalyticsExportTemplate[property_status].xlsx
@@ -43,46 +43,46 @@
     <t xml:space="preserve">New or reopened</t>
   </si>
   <si>
-    <t xml:space="preserve">{d.ticket[i].address}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].processing}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].completed}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].canceled}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].deferred}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].closed}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i].new_or_reopened}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].address}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].processing}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].completed}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].canceled}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].deferred}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].closed}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d.ticket[i + 1].new_or_reopened}</t>
+    <t xml:space="preserve">{d.tickets[i].address}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].processing}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].completed}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].canceled}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].deferred}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].closed}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i].new_or_reopened}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].address}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].processing}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].completed}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].canceled}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].deferred}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].closed}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d.tickets[i + 1].new_or_reopened}</t>
   </si>
 </sst>
 </file>
@@ -288,10 +288,10 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.09"/>

</xml_diff>